<commit_message>
bijna hele website responsive gemaakt
</commit_message>
<xml_diff>
--- a/pakketten.xlsx
+++ b/pakketten.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Kolom4</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>€10 Per Maand</t>
+  </si>
+  <si>
+    <t>512 MB Ram</t>
+  </si>
+  <si>
+    <t>100 GB Dataverkeer Per maand</t>
+  </si>
+  <si>
+    <t>5,95 Per Maand</t>
   </si>
 </sst>
 </file>
@@ -261,42 +270,42 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F958345-71D9-428B-AC09-814D22BB3283}" name="Tabel2" displayName="Tabel2" ref="A9:B10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F958345-71D9-428B-AC09-814D22BB3283}" name="Tabel2" displayName="Tabel2" ref="A9:B10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A9:B10" xr:uid="{17EC5B87-8437-4C88-9769-E092F89A3784}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A2A23A87-0B97-4464-A34F-8FD1D77D8F7C}" name="Pakket Geel" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D79A7FA6-12FC-4E5C-AE33-C2503016BADC}" name=" " dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{A2A23A87-0B97-4464-A34F-8FD1D77D8F7C}" name="Pakket Geel" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D79A7FA6-12FC-4E5C-AE33-C2503016BADC}" name=" " dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{750E7410-92FD-4535-BA31-C7EF159D046F}" name="Tabel3" displayName="Tabel3" ref="A11:B12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{750E7410-92FD-4535-BA31-C7EF159D046F}" name="Tabel3" displayName="Tabel3" ref="A11:B12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A11:B12" xr:uid="{1CA148AE-8BD9-448C-A43F-36C894C38F9C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E6BD5B71-3EBA-4568-A484-03E585D67E13}" name="Pakket Oranje" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{58717A82-2CE4-406F-864D-5D2B9B86BC8A}" name=" " dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{E6BD5B71-3EBA-4568-A484-03E585D67E13}" name="Pakket Oranje" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{58717A82-2CE4-406F-864D-5D2B9B86BC8A}" name=" " dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1115B9B0-EB6F-4D42-B4FA-8361DF9F018A}" name="Tabel4" displayName="Tabel4" ref="A13:B14" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1115B9B0-EB6F-4D42-B4FA-8361DF9F018A}" name="Tabel4" displayName="Tabel4" ref="A13:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A13:B14" xr:uid="{7A21A3D1-0BD1-41B7-8828-2AB214114F52}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F75D8795-98F2-4926-8BC0-04C87BF9EDB3}" name="Pakket Groen" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{3458501E-3C9B-458D-A0F9-38112A2B2DF0}" name=" " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F75D8795-98F2-4926-8BC0-04C87BF9EDB3}" name="Pakket Groen" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3458501E-3C9B-458D-A0F9-38112A2B2DF0}" name=" " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CD5CC1-6B3C-43D0-B6B0-082061E546E8}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,6 +747,36 @@
         <v>31</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>